<commit_message>
Updated rubric / clean-up
</commit_message>
<xml_diff>
--- a/ProjectImplementationRubric.xlsx
+++ b/ProjectImplementationRubric.xlsx
@@ -1,37 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Repos\CS297-CourseMaterials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS297-CourseMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC03E7AC-7413-431B-9CE5-45DA1855EA8C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBABF8D3-9E04-1D4B-91A5-DB374EC47A52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18480" yWindow="3630" windowWidth="17970" windowHeight="10470" xr2:uid="{5001B676-3EE2-41FC-AE2E-35CDF19EF21D}"/>
+    <workbookView xWindow="13200" yWindow="3520" windowWidth="12200" windowHeight="10480" xr2:uid="{5001B676-3EE2-41FC-AE2E-35CDF19EF21D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Capstone Project Implementation Rubric</t>
   </si>
@@ -76,6 +70,12 @@
   </si>
   <si>
     <t>Possible</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Completeness of functional testing</t>
   </si>
 </sst>
 </file>
@@ -468,25 +468,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47327E91-177B-4428-A352-1A16E02A04A8}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.21875" customWidth="1"/>
-    <col min="2" max="2" width="7.77734375" customWidth="1"/>
-    <col min="3" max="3" width="2.44140625" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" customWidth="1"/>
+    <col min="3" max="3" width="2.5" customWidth="1"/>
+    <col min="7" max="7" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
@@ -495,46 +496,54 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>10</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="D11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>25</v>
       </c>
@@ -542,29 +551,38 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D14" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <f>SUM(B4:B18)</f>
+        <v>100</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reset back to the commit from the other computer
</commit_message>
<xml_diff>
--- a/ProjectImplementationRubric.xlsx
+++ b/ProjectImplementationRubric.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t xml:space="preserve">Capstone Project Implementation Rubric</t>
   </si>
@@ -84,6 +84,45 @@
   </si>
   <si>
     <t xml:space="preserve">Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See below</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A few category comments, no explanatory comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No unit tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The only major features completed were the metronome and events.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code quality issues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">passwords in source code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unused dBcontext field in multiple controllers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple html validation errors in the views</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Models:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iresources is not an interface and is not used</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HtmlForm and HtmlHero files con’t match class names with VM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inconsistent indentation with [key] attribute</t>
   </si>
 </sst>
 </file>
@@ -99,7 +138,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -122,7 +160,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -131,7 +168,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -139,21 +175,18 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -161,7 +194,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -170,14 +202,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -185,7 +215,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -230,56 +259,60 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -338,14 +371,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -353,67 +386,25 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -432,35 +423,11 @@
           <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
@@ -475,113 +442,117 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I21" activeCellId="1" sqref="D22:D28 I21"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="1.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="1.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.44"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="4" t="s">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="0" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="0" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C9" s="4" t="s">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4" t="s">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="0" t="s">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="0" t="s">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="0" t="s">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="0" t="s">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
         <f aca="false">SUM(A4:A18)</f>
         <v>70</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -601,177 +572,233 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22:D28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="1.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="1.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.44"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="3" t="s">
+      <c r="A4" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="8"/>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="9"/>
+      <c r="D5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="8"/>
-      <c r="D6" s="10" t="s">
+      <c r="E5" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="9"/>
+      <c r="D6" s="11" t="s">
         <v>4</v>
       </c>
+      <c r="E6" s="10" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="8"/>
-      <c r="D7" s="10" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="11" t="s">
         <v>5</v>
       </c>
+      <c r="E7" s="10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="8"/>
+      <c r="C8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="4" t="s">
+      <c r="A9" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="E9" s="10" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="4" t="s">
+      <c r="A10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="E10" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="9"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="8"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B13" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="3" t="s">
+      <c r="C13" s="9"/>
+      <c r="D13" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="8"/>
-      <c r="D14" s="11" t="s">
+      <c r="C14" s="9"/>
+      <c r="D14" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="8"/>
-      <c r="D15" s="10" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="8"/>
-      <c r="D16" s="10" t="s">
+      <c r="C16" s="9"/>
+      <c r="D16" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="8"/>
-      <c r="D17" s="10" t="s">
+      <c r="C17" s="9"/>
+      <c r="D17" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="8"/>
-      <c r="D18" s="10" t="s">
+      <c r="C18" s="9"/>
+      <c r="D18" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="1" t="n">
         <f aca="false">SUM(A4:A18)</f>
         <v>70</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <f aca="false">SUM(B4:B18)</f>
-        <v>70</v>
-      </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="10" t="n">
-        <f aca="false">B20/A20</f>
-        <v>1</v>
+      <c r="E20" s="11"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D22" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D23" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D25" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D26" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D27" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D28" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D29" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>